<commit_message>
Add new chaps for Multitenancy and LoadBalancing
</commit_message>
<xml_diff>
--- a/misc/tracking-list.xlsx
+++ b/misc/tracking-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DISK D\Projects\#R&amp;D\MkDocs\SmartWebDoc-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\smartsysbg\SmartWebDoc\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24987E05-8335-4876-B5EB-5F0F76C0E62D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5136028-BFDF-4ED3-9266-1028C6F7AE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>access-to-opc-data.md</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>hmi-editor-mastering.md</t>
+  </si>
+  <si>
+    <t>multitenancy.md</t>
+  </si>
+  <si>
+    <t>load-balancing.md</t>
   </si>
 </sst>
 </file>
@@ -997,9 +1003,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1205,19 +1213,15 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>38</v>
@@ -1229,27 +1233,27 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1257,15 +1261,19 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1273,21 +1281,15 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1295,47 +1297,53 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1343,19 +1351,15 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1363,31 +1367,51 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{3EB53D06-933D-44D4-B513-4BE5F8681C84}"/>

</xml_diff>

<commit_message>
Small chages to Load Balancing chapter and other
</commit_message>
<xml_diff>
--- a/misc/tracking-list.xlsx
+++ b/misc/tracking-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\smartsysbg\SmartWebDoc\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15EE1F-4107-4BE2-932E-CAB54F2B54BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A8DF5-106A-466D-8F6A-436D17734F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32355" yWindow="1965" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
   <si>
     <t>access-to-opc-data.md</t>
   </si>
@@ -1005,9 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1221,9 +1219,15 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">

</xml_diff>

<commit_message>
Users and Roles chapter compleated
</commit_message>
<xml_diff>
--- a/misc/tracking-list.xlsx
+++ b/misc/tracking-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\smartsysbg\SmartWebDoc\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34326A8A-74D3-45E1-99C5-A75102D91EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DBCB88-8E8C-4DCC-ACFA-A4F5CD7EF1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="990" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1560" windowWidth="27780" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
   <si>
     <t>access-to-opc-data.md</t>
   </si>
@@ -1005,9 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1401,9 +1399,15 @@
       <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">

</xml_diff>